<commit_message>
Logic for creating folders and moving files
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/config.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6B04F5-AE36-4EDF-8BF9-7A9CE7872CB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152834CA-174A-4E53-9377-5AC68F5EB8A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="3735" windowWidth="18750" windowHeight="7215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -215,7 +215,16 @@
     <t>Inbox\CoFS\Robot in-box\Robot Exceptions</t>
   </si>
   <si>
-    <t>C:\Users\{0}\Desktop\RobotWorkingFolder\</t>
+    <t>\\nevmfil001\on\BRANCHB\CERTIFICATES OF FREE SALE\E-MAIL APPLICATIONS\</t>
+  </si>
+  <si>
+    <t>EmailApplicationsFolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folder Path for the email applications folder on shared drive. </t>
+  </si>
+  <si>
+    <t>\Desktop\RobotWorkingFolder\</t>
   </si>
 </sst>
 </file>
@@ -342,8 +351,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C33" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -650,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,67 +909,78 @@
         <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes to proxy main logic for logging parent cases. Added in remaining sprint1 workflows
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/config.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152834CA-174A-4E53-9377-5AC68F5EB8A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8699B854-4A71-4C29-B162-9BAA48E825B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="3735" windowWidth="18750" windowHeight="7215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="3735" windowWidth="18750" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -662,7 +662,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Final sprint1 stories and start of reading word application. WordVB library added
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/config.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/config.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8699B854-4A71-4C29-B162-9BAA48E825B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02B5C1D-BCE2-4BBF-BC45-856837D08D87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="3735" windowWidth="18750" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13605" yWindow="1125" windowWidth="18750" windowHeight="10755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ApplicationFields" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="149">
   <si>
     <t>Name</t>
   </si>
@@ -215,9 +216,6 @@
     <t>Inbox\CoFS\Robot in-box\Robot Exceptions</t>
   </si>
   <si>
-    <t>\\nevmfil001\on\BRANCHB\CERTIFICATES OF FREE SALE\E-MAIL APPLICATIONS\</t>
-  </si>
-  <si>
     <t>EmailApplicationsFolder</t>
   </si>
   <si>
@@ -225,6 +223,264 @@
   </si>
   <si>
     <t>\Desktop\RobotWorkingFolder\</t>
+  </si>
+  <si>
+    <t>\\EARTH.GSI.GOV.UK\USER\SHARED\Agency\CoFS for G drive\</t>
+  </si>
+  <si>
+    <t>PartA</t>
+  </si>
+  <si>
+    <t>PartB</t>
+  </si>
+  <si>
+    <t>PartC</t>
+  </si>
+  <si>
+    <t>PartD</t>
+  </si>
+  <si>
+    <t>PartE</t>
+  </si>
+  <si>
+    <t>PartF</t>
+  </si>
+  <si>
+    <t>PartG</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>ACompName1</t>
+  </si>
+  <si>
+    <t>CompanyAddress</t>
+  </si>
+  <si>
+    <t>CompanyPostcode</t>
+  </si>
+  <si>
+    <t>PostalCompName</t>
+  </si>
+  <si>
+    <t>PostalCompAddress</t>
+  </si>
+  <si>
+    <t>PostalCompPostcode</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>ContactPhone</t>
+  </si>
+  <si>
+    <t>ContactEmail</t>
+  </si>
+  <si>
+    <t>ACompAddress1</t>
+  </si>
+  <si>
+    <t>ACompPostcode1</t>
+  </si>
+  <si>
+    <t>Acompnameifdiff</t>
+  </si>
+  <si>
+    <t>AAddressIfDiff</t>
+  </si>
+  <si>
+    <t>ApostcodeIfDiff</t>
+  </si>
+  <si>
+    <t>AConName</t>
+  </si>
+  <si>
+    <t>AConTel</t>
+  </si>
+  <si>
+    <t>AConEmail</t>
+  </si>
+  <si>
+    <t>ApplicantName</t>
+  </si>
+  <si>
+    <t>ApplicantPosition</t>
+  </si>
+  <si>
+    <t>ApplicantCompany</t>
+  </si>
+  <si>
+    <t>Gcompanyname</t>
+  </si>
+  <si>
+    <t>GPosition</t>
+  </si>
+  <si>
+    <t>GNameBLOCK</t>
+  </si>
+  <si>
+    <t>Signature</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>FSpan</t>
+  </si>
+  <si>
+    <t>FEng</t>
+  </si>
+  <si>
+    <t>Fyesorig</t>
+  </si>
+  <si>
+    <t>ESoE</t>
+  </si>
+  <si>
+    <t>ScheduleOA</t>
+  </si>
+  <si>
+    <t>MarksAndNumbers</t>
+  </si>
+  <si>
+    <t>NoPackages</t>
+  </si>
+  <si>
+    <t>ProductDetails</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ProductList</t>
+  </si>
+  <si>
+    <t>CConsigneeName</t>
+  </si>
+  <si>
+    <t>CDestinationCountry</t>
+  </si>
+  <si>
+    <t>DConsigneeName</t>
+  </si>
+  <si>
+    <t>DDestinationCountry</t>
+  </si>
+  <si>
+    <t>DAdditionalHeader</t>
+  </si>
+  <si>
+    <t>DAdditionalDetails</t>
+  </si>
+  <si>
+    <t>CAdditionalDetails</t>
+  </si>
+  <si>
+    <t>CAdditionalHeader</t>
+  </si>
+  <si>
+    <t>FreeSaleStandard</t>
+  </si>
+  <si>
+    <t>ManFreeSale</t>
+  </si>
+  <si>
+    <t>DecOrigin</t>
+  </si>
+  <si>
+    <t>HumanConsumption</t>
+  </si>
+  <si>
+    <t>FreeSaleAlcohol</t>
+  </si>
+  <si>
+    <t>FreeSaleAnimal</t>
+  </si>
+  <si>
+    <t>ManFreeAnimal</t>
+  </si>
+  <si>
+    <t>NonMammalian</t>
+  </si>
+  <si>
+    <t>NonAnimal</t>
+  </si>
+  <si>
+    <t>DioxinFree</t>
+  </si>
+  <si>
+    <t>BDioxFree</t>
+  </si>
+  <si>
+    <t>BNonAn</t>
+  </si>
+  <si>
+    <t>BNonMam</t>
+  </si>
+  <si>
+    <t>BMandFSaleAF</t>
+  </si>
+  <si>
+    <t>BFSaleAF</t>
+  </si>
+  <si>
+    <t>BFSAlc</t>
+  </si>
+  <si>
+    <t>BHumCons</t>
+  </si>
+  <si>
+    <t>BDecOrig</t>
+  </si>
+  <si>
+    <t>BMandFS</t>
+  </si>
+  <si>
+    <t>BFSS</t>
+  </si>
+  <si>
+    <t>CProdname</t>
+  </si>
+  <si>
+    <t>CSepCerts</t>
+  </si>
+  <si>
+    <t>Dropdown1</t>
+  </si>
+  <si>
+    <t>CAddDetails</t>
+  </si>
+  <si>
+    <t>CCosigneeName</t>
+  </si>
+  <si>
+    <t>CDestCount</t>
+  </si>
+  <si>
+    <t>DMandN</t>
+  </si>
+  <si>
+    <t>DNoPack</t>
+  </si>
+  <si>
+    <t>DProdDets</t>
+  </si>
+  <si>
+    <t>Dropdown2</t>
+  </si>
+  <si>
+    <t>DadditionalDeets</t>
+  </si>
+  <si>
+    <t>DCosigneeAdd2</t>
+  </si>
+  <si>
+    <t>DDestinCount</t>
   </si>
 </sst>
 </file>
@@ -306,7 +562,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -351,12 +637,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C33" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C33" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:C33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB8025D7-5F6D-42D1-8C47-07CA584992D5}" name="Table13" displayName="Table13" ref="A1:C47" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C47" xr:uid="{56FE7331-7682-4204-88E6-48966BDA92CC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B7EB075A-3644-4077-908D-24FFC60E5632}" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{A6E5FDC3-8203-4F08-B989-D2E6D7575FC6}" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{B31D32FF-9F7D-4C20-877B-68A72A6F72ED}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -661,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +1207,7 @@
         <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>47</v>
@@ -917,13 +1215,13 @@
     </row>
     <row r="25" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,4 +1289,438 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A44EFD-45F3-423F-B2B0-CF6CEF7186D6}">
+  <dimension ref="A1:C47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="4"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added country look up list and journey testing to bp2
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/config.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02B5C1D-BCE2-4BBF-BC45-856837D08D87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2807D4-9404-441B-A93A-B236D3F4ED74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13605" yWindow="1125" windowWidth="18750" windowHeight="10755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="152">
   <si>
     <t>Name</t>
   </si>
@@ -481,6 +481,15 @@
   </si>
   <si>
     <t>DDestinCount</t>
+  </si>
+  <si>
+    <t>CountryLookUpPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File path for Excel doc containing valid countries for certificates to be sent to. Stored in the shared drive. </t>
+  </si>
+  <si>
+    <t>\\EARTH.GSI.GOV.UK\USER\SHARED\Agency\CoFS for G drive\RobotDocuments\ValidCountriesList.xlsx</t>
   </si>
 </sst>
 </file>
@@ -637,8 +646,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C33" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:C33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C34" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="6"/>
@@ -957,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,61 +1233,72 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1295,7 +1315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A44EFD-45F3-423F-B2B0-CF6CEF7186D6}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
End of sprint 2, finished validating application form
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/config.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80BA1D5-A27B-408C-95E8-7B7DAD11676C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BD9034-0BA8-4072-9352-FE150DE1FEB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="4170" windowWidth="19320" windowHeight="9750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1316,7 +1316,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
End of sprint 3 dev stories, added values to enterCertDetails
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/config.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54D4E3E-FE28-4FBB-A166-359751E8BEFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF2EB9D-C9A0-46D3-B33D-D19E09DB88FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1095" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="188">
   <si>
     <t>Name</t>
   </si>
@@ -516,9 +516,6 @@
     <t>Packages</t>
   </si>
   <si>
-    <t>Schedule of Analysis</t>
-  </si>
-  <si>
     <t>TRD</t>
   </si>
   <si>
@@ -595,13 +592,19 @@
   </si>
   <si>
     <t>NumberOfCopiesHere</t>
+  </si>
+  <si>
+    <t>SpanishHeaders</t>
+  </si>
+  <si>
+    <t>ScheduleofAnalysis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,32 +630,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -674,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -698,17 +675,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,8 +754,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C50" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:C50" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C55" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="6"/>
@@ -1108,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,13 +1343,13 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1410,13 +1376,13 @@
     </row>
     <row r="29" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1483,37 +1449,37 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B41" s="11" t="s">
-        <v>169</v>
+      <c r="B41" s="4" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1521,7 +1487,7 @@
         <v>158</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1529,62 +1495,67 @@
         <v>159</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="13" t="s">
-        <v>180</v>
+      <c r="B45" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B50" s="4" t="s">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>186</v>
       </c>
     </row>

</xml_diff>

<commit_message>
journey testing - changes for spanish cert filepaths, added sep cert user input
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/config.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF2EB9D-C9A0-46D3-B33D-D19E09DB88FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5334683B-6B77-47DA-B25E-350B8CEDBF04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="190">
   <si>
     <t>Name</t>
   </si>
@@ -594,10 +594,16 @@
     <t>NumberOfCopiesHere</t>
   </si>
   <si>
-    <t>SpanishHeaders</t>
-  </si>
-  <si>
     <t>ScheduleofAnalysis</t>
+  </si>
+  <si>
+    <t>Regex</t>
+  </si>
+  <si>
+    <t>SeparateProducts</t>
+  </si>
+  <si>
+    <t>{\Wproduct\W:\W(\d+\s*)+\W}</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,7 +1522,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>178</v>
@@ -1556,7 +1562,15 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing, updated form, added breakpoint 5, fixed sep certs logic
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/config.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5334683B-6B77-47DA-B25E-350B8CEDBF04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6ECDFAA-EC4A-40DF-BE0F-9333792493A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="193">
   <si>
     <t>Name</t>
   </si>
@@ -604,6 +604,15 @@
   </si>
   <si>
     <t>{\Wproduct\W:\W(\d+\s*)+\W}</t>
+  </si>
+  <si>
+    <t>AddressLabelPath</t>
+  </si>
+  <si>
+    <t>\\EARTH.GSI.GOV.UK\USER\SHARED\Agency\CoFS for G drive\RobotDocuments\RobotAddressLabelTemplate.docx</t>
+  </si>
+  <si>
+    <t>{\Wproduct\W:\W((\w+\s*\W)+)}</t>
   </si>
 </sst>
 </file>
@@ -760,8 +769,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C55" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:C55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C56" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C56" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="6"/>
@@ -1080,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,183 +1402,194 @@
     </row>
     <row r="30" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>167</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>70</v>
+        <v>160</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>186</v>
+        <v>70</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>189</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Address check now using forms
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/config.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD4C094-B650-4DB6-A444-53B981DDE968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4FF09F-A38C-4277-8511-0BFEBE4CEE64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="197">
   <si>
     <t>Name</t>
   </si>
@@ -615,8 +615,16 @@
     <t>{\W{0,2}product\W{0,2}:\W{0,2}([^(},{)]+)</t>
   </si>
   <si>
-    <t>{\Wproduct\W:\W(.+)\W} 
-{\W{0,2}product\W{0,2}:\W{0,2}(.+)\W},</t>
+    <t>AddressContinueRegex</t>
+  </si>
+  <si>
+    <t>AddressRegex</t>
+  </si>
+  <si>
+    <t>\WContinue\W:(\w+)</t>
+  </si>
+  <si>
+    <t>{\WIN_strAddressLabel\W:\W([^(},{)]+)</t>
   </si>
 </sst>
 </file>
@@ -1093,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,9 +1605,20 @@
         <v>191</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="C54" s="4" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>193</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes made for demo recording - Laura last push before leaving
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/config.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0377A124-97E6-4EB7-B6FC-20580D32FB59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBC3F8F-00BC-4E4F-9588-C0D250D2D90E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16830" yWindow="4620" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,16 +621,16 @@
     <t>IN_strAddressLabel\W{0,2}:\W{0,2}(.+)",</t>
   </si>
   <si>
-    <t>Laura.Battell@defra.gov.uk</t>
-  </si>
-  <si>
     <t>C:\Users\x953922\Desktop\CoFS\To Be Printed\</t>
   </si>
   <si>
-    <t>C:\Users\x953922\Desktop\CoFS\Robot Certificate Templates\</t>
-  </si>
-  <si>
     <t>C:\Users\x953922\Desktop\CoFS\</t>
+  </si>
+  <si>
+    <t>\\EARTH.GSI.GOV.UK\USER\SHARED\Agency\CoFS for G drive\RobotDocuments\Robot Certificate Templates\</t>
+  </si>
+  <si>
+    <t>Trader@rpa.gov.uk</t>
   </si>
 </sst>
 </file>
@@ -1109,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,7 +1173,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>33</v>
@@ -1390,7 +1390,7 @@
         <v>57</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>58</v>
@@ -1412,7 +1412,7 @@
         <v>161</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>162</v>
@@ -1447,7 +1447,7 @@
         <v>46</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>52</v>

</xml_diff>